<commit_message>
adding more time effort
</commit_message>
<xml_diff>
--- a/docs/Burndown/Burndown.xlsx
+++ b/docs/Burndown/Burndown.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\api-6-semestre\docs\management\Burndown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\api-6-semestre\docs\Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5F4CFA-E31E-4E12-B793-E3515A79CC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23174667-6673-4D0C-A142-9ACF3760AEFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,7 +182,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -194,6 +194,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -271,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,6 +329,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,16 +630,16 @@
                   <c:v>18.260000000000005</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18.260000000000005</c:v>
+                  <c:v>16.260000000000005</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18.260000000000005</c:v>
+                  <c:v>16.260000000000005</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>18.260000000000005</c:v>
+                  <c:v>16.260000000000005</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18.260000000000005</c:v>
+                  <c:v>16.260000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -845,28 +853,28 @@
                   <c:v>57.142857142857189</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>70.000000000000043</c:v>
+                  <c:v>50.000000000000043</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>62.857142857142897</c:v>
+                  <c:v>42.857142857142897</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>55.714285714285751</c:v>
+                  <c:v>35.714285714285751</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>48.571428571428605</c:v>
+                  <c:v>28.571428571428608</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41.428571428571459</c:v>
+                  <c:v>21.428571428571466</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>34.285714285714313</c:v>
+                  <c:v>24.285714285714324</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>27.142857142857171</c:v>
+                  <c:v>17.142857142857181</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20.000000000000028</c:v>
+                  <c:v>10.000000000000039</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1771,15 +1779,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>160413</xdr:colOff>
+      <xdr:colOff>217563</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2124,11 +2132,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B4BA60-9604-4D54-BDB3-BA720851CBCD}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2546,7 +2554,7 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" si="0"/>
-        <v>2.33</v>
+        <v>4.33</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -2568,7 +2576,9 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
+      <c r="T11" s="3">
+        <v>2</v>
+      </c>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
@@ -2728,19 +2738,19 @@
       </c>
       <c r="T14" s="3">
         <f t="shared" si="1"/>
-        <v>18.260000000000005</v>
+        <v>16.260000000000005</v>
       </c>
       <c r="U14" s="3">
         <f t="shared" si="1"/>
-        <v>18.260000000000005</v>
+        <v>16.260000000000005</v>
       </c>
       <c r="V14" s="3">
         <f t="shared" si="1"/>
-        <v>18.260000000000005</v>
+        <v>16.260000000000005</v>
       </c>
       <c r="W14" s="3">
         <f t="shared" si="1"/>
-        <v>18.260000000000005</v>
+        <v>16.260000000000005</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
@@ -2792,7 +2802,7 @@
         <v>78.571428571428612</v>
       </c>
       <c r="M15" s="3">
-        <f>L15-B20</f>
+        <f>(L15-B20)</f>
         <v>71.428571428571473</v>
       </c>
       <c r="N15" s="3">
@@ -2800,40 +2810,40 @@
         <v>64.285714285714334</v>
       </c>
       <c r="O15" s="3">
-        <f>N15-B20</f>
+        <f>(N15-B20)</f>
         <v>57.142857142857189</v>
       </c>
       <c r="P15" s="3">
-        <f>(O15-B20) + 20</f>
-        <v>70.000000000000043</v>
+        <f>(O15-B20)</f>
+        <v>50.000000000000043</v>
       </c>
       <c r="Q15" s="3">
         <f>P15-B20</f>
-        <v>62.857142857142897</v>
+        <v>42.857142857142897</v>
       </c>
       <c r="R15" s="3">
         <f>Q15-B20</f>
-        <v>55.714285714285751</v>
+        <v>35.714285714285751</v>
       </c>
       <c r="S15" s="3">
         <f>R15-B20</f>
-        <v>48.571428571428605</v>
+        <v>28.571428571428608</v>
       </c>
       <c r="T15" s="3">
         <f>S15-B20</f>
-        <v>41.428571428571459</v>
+        <v>21.428571428571466</v>
       </c>
       <c r="U15" s="3">
-        <f>T15-B20</f>
-        <v>34.285714285714313</v>
+        <f>(T15-B20) + 10</f>
+        <v>24.285714285714324</v>
       </c>
       <c r="V15" s="3">
         <f>U15-B20</f>
-        <v>27.142857142857171</v>
+        <v>17.142857142857181</v>
       </c>
       <c r="W15" s="3">
         <f>IF(V15-B20&lt;0,0,V15-B20)</f>
-        <v>20.000000000000028</v>
+        <v>10.000000000000039</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2861,6 +2871,9 @@
         <f>B15/B18</f>
         <v>7.1428571428571432</v>
       </c>
+    </row>
+    <row r="35" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S35" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
creating sprint 2 burndown
</commit_message>
<xml_diff>
--- a/docs/Burndown/Burndown.xlsx
+++ b/docs/Burndown/Burndown.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\api-6-semestre\docs\Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332336B3-E6E7-43B5-B09D-E0304400C858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D56A526-FD05-4C63-9A44-DE051E9AF83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tempo" sheetId="3" r:id="rId1"/>
-    <sheet name="Sprint 0" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 2" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t>Atividades</t>
   </si>
@@ -436,7 +437,7 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Sprint 0'!$C$2:$W$3</c:f>
+              <c:f>'Sprint 1'!$C$2:$W$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="21"/>
                 <c:lvl>
@@ -574,7 +575,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 0'!$C$14:$W$14</c:f>
+              <c:f>'Sprint 1'!$C$14:$W$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -671,7 +672,7 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Sprint 0'!$C$2:$W$3</c:f>
+              <c:f>'Sprint 1'!$C$2:$W$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="21"/>
                 <c:lvl>
@@ -809,7 +810,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 0'!$C$15:$W$15</c:f>
+              <c:f>'Sprint 1'!$C$15:$W$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -883,6 +884,877 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-450B-49C5-8FA6-216D256F23DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1762041440"/>
+        <c:axId val="1762034784"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1762041440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Dias da Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1762034784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1762034784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Quantidade de</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t> esforço</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1762041440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx2"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Burndown</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Real</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Sprint 2'!$C$2:$W$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="21"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>11</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>12</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>13</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>14</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>17</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>18</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>19</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>21</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>29/08</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>30/08</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>31/08</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>01/09</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>02/09</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>03/09</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>04/09</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>05/09</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>06/09</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>07/09</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>08/09</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>09/09</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>10/09</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>11/09</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>12/09</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>13/09</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>14/09</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>15/09</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>16/09</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>17/09</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>18/09</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$C$14:$W$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AF68-4E62-92E0-DD3A7A958ADA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Sprint 2'!$C$2:$W$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="21"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>11</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>12</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>13</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>14</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>17</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>18</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>19</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>21</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>29/08</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>30/08</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>31/08</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>01/09</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>02/09</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>03/09</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>04/09</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>05/09</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>06/09</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>07/09</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>08/09</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>09/09</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>10/09</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>11/09</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>12/09</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>13/09</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>14/09</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>15/09</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>16/09</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>17/09</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>18/09</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$C$15:$W$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>152.38095238095238</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>144.76190476190476</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>137.14285714285714</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>129.52380952380952</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>121.9047619047619</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>114.28571428571428</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>99.047619047619037</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>91.428571428571416</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>83.809523809523796</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>76.190476190476176</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>68.571428571428555</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60.952380952380935</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>53.333333333333314</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45.714285714285694</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>38.095238095238074</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30.476190476190453</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22.857142857142833</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15.238095238095214</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.6190476190475955</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AF68-4E62-92E0-DD3A7A958ADA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1258,7 +2130,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1799,6 +3227,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>195151</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>141194</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>520513</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>93569</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05384D09-DB17-413E-89C5-6C48CF626F8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2134,7 +3605,7 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="T30" sqref="T30"/>
     </sheetView>
@@ -2895,4 +4366,717 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F09A8E-961C-4A18-A039-5BA904275A7B}">
+  <dimension ref="A1:W35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R26" sqref="R26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2">
+        <v>8</v>
+      </c>
+      <c r="K3" s="2">
+        <v>9</v>
+      </c>
+      <c r="L3" s="2">
+        <v>10</v>
+      </c>
+      <c r="M3" s="2">
+        <v>11</v>
+      </c>
+      <c r="N3" s="2">
+        <v>12</v>
+      </c>
+      <c r="O3" s="2">
+        <v>13</v>
+      </c>
+      <c r="P3" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>15</v>
+      </c>
+      <c r="R3" s="2">
+        <v>16</v>
+      </c>
+      <c r="S3" s="2">
+        <v>17</v>
+      </c>
+      <c r="T3" s="2">
+        <v>18</v>
+      </c>
+      <c r="U3" s="2">
+        <v>19</v>
+      </c>
+      <c r="V3" s="2">
+        <v>20</v>
+      </c>
+      <c r="W3" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f>SUM(C4:W4)</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" ref="B5:B13" si="0">SUM(C5:W5)</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="5">
+        <f>B15</f>
+        <v>160</v>
+      </c>
+      <c r="C14" s="3">
+        <f>B15-SUM(C4:C13)</f>
+        <v>160</v>
+      </c>
+      <c r="D14" s="3">
+        <f>C14-SUM(D4:D13)</f>
+        <v>160</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" ref="E14:W14" si="1">D14-SUM(E4:E13)</f>
+        <v>160</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="O14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="P14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="Q14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="R14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="S14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="T14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="U14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="V14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="W14" s="3">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="10">
+        <f>Tempo!B4</f>
+        <v>160</v>
+      </c>
+      <c r="C15" s="3">
+        <f>B15-B20</f>
+        <v>152.38095238095238</v>
+      </c>
+      <c r="D15" s="3">
+        <f>C15-B20</f>
+        <v>144.76190476190476</v>
+      </c>
+      <c r="E15" s="3">
+        <f>D15-B20</f>
+        <v>137.14285714285714</v>
+      </c>
+      <c r="F15" s="3">
+        <f>E15-B20</f>
+        <v>129.52380952380952</v>
+      </c>
+      <c r="G15" s="3">
+        <f>F15-B20</f>
+        <v>121.9047619047619</v>
+      </c>
+      <c r="H15" s="3">
+        <f>G15-B20</f>
+        <v>114.28571428571428</v>
+      </c>
+      <c r="I15" s="3">
+        <f>H15-B20</f>
+        <v>106.66666666666666</v>
+      </c>
+      <c r="J15" s="3">
+        <f>I15-B20</f>
+        <v>99.047619047619037</v>
+      </c>
+      <c r="K15" s="3">
+        <f>J15-B20</f>
+        <v>91.428571428571416</v>
+      </c>
+      <c r="L15" s="3">
+        <f>K15-B20</f>
+        <v>83.809523809523796</v>
+      </c>
+      <c r="M15" s="3">
+        <f>(L15-B20)</f>
+        <v>76.190476190476176</v>
+      </c>
+      <c r="N15" s="3">
+        <f>M15-B20</f>
+        <v>68.571428571428555</v>
+      </c>
+      <c r="O15" s="3">
+        <f>(N15-B20)</f>
+        <v>60.952380952380935</v>
+      </c>
+      <c r="P15" s="3">
+        <f>(O15-B20)</f>
+        <v>53.333333333333314</v>
+      </c>
+      <c r="Q15" s="3">
+        <f>P15-B20</f>
+        <v>45.714285714285694</v>
+      </c>
+      <c r="R15" s="3">
+        <f>Q15-B20</f>
+        <v>38.095238095238074</v>
+      </c>
+      <c r="S15" s="3">
+        <f>R15-B20</f>
+        <v>30.476190476190453</v>
+      </c>
+      <c r="T15" s="3">
+        <f>S15-B20</f>
+        <v>22.857142857142833</v>
+      </c>
+      <c r="U15" s="3">
+        <f>(T15-B20)</f>
+        <v>15.238095238095214</v>
+      </c>
+      <c r="V15" s="3">
+        <f>U15-B20</f>
+        <v>7.6190476190475955</v>
+      </c>
+      <c r="W15" s="3">
+        <f>IF(V15-B20&lt;0,0,V15-B20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" s="14"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="12">
+        <f>COUNTA(C3:W3)</f>
+        <v>21</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="11"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="9">
+        <f>B15/B18</f>
+        <v>7.6190476190476186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R32" s="16"/>
+    </row>
+    <row r="35" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S35" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:W1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
initial sprint 3 burndown
</commit_message>
<xml_diff>
--- a/docs/Burndown/Burndown.xlsx
+++ b/docs/Burndown/Burndown.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\api-6-semestre\docs\Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C386B2D9-73C6-4BCA-AA00-9D2A04427EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DD2410-9051-4C74-AE2F-4702023EEFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tempo" sheetId="3" r:id="rId1"/>
     <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 2" sheetId="6" r:id="rId3"/>
+    <sheet name="Sprint 3" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
   <si>
     <t>Atividades</t>
   </si>
@@ -2159,6 +2160,872 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Burndown</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Real</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Sprint 3'!$C$2:$W$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="21"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>11</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>12</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>13</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>14</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>17</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>18</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>19</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>21</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>19/09</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>20/09</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>21/09</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>22/09</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>23/09</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>24/09</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>25/09</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>26/09</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>27/09</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>28/09</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>29/09</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>30/09</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>01/10</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>02/10</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>03/10</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>04/10</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>05/10</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>06/10</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>07/10</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>08/10</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>09/10</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 3'!$C$14:$W$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B186-4CE2-95EE-205B5A8FD00E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Sprint 3'!$C$2:$W$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="21"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>11</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>12</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>13</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>14</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>17</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>18</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>19</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>21</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>19/09</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>20/09</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>21/09</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>22/09</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>23/09</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>24/09</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>25/09</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>26/09</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>27/09</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>28/09</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>29/09</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>30/09</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>01/10</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>02/10</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>03/10</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>04/10</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>05/10</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>06/10</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>07/10</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>08/10</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>09/10</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 3'!$C$15:$W$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>133.33333333333334</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>126.66666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>113.33333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>106.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.999999999999986</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>93.333333333333314</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>86.666666666666643</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>79.999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>73.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>66.666666666666629</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59.999999999999964</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>53.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>46.666666666666636</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39.999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>33.333333333333307</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>26.666666666666639</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19.999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13.333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.6666666666666368</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B186-4CE2-95EE-205B5A8FD00E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1762041440"/>
+        <c:axId val="1762034784"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1762041440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1762034784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1762034784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Effort</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1762041440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx2"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2239,6 +3106,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2756,6 +3663,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3333,6 +4756,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05384D09-DB17-413E-89C5-6C48CF626F8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>113154</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>101144</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>438516</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>44750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B30DB901-65E2-4805-B3C1-81568357E2DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4523,7 +5989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F09A8E-961C-4A18-A039-5BA904275A7B}">
   <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="W20" sqref="W20"/>
     </sheetView>
@@ -5353,4 +6819,728 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34691D87-3A65-488E-9A9A-734FA0D4B672}">
+  <dimension ref="A1:W35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C47" sqref="C47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2">
+        <v>8</v>
+      </c>
+      <c r="K3" s="2">
+        <v>9</v>
+      </c>
+      <c r="L3" s="2">
+        <v>10</v>
+      </c>
+      <c r="M3" s="2">
+        <v>11</v>
+      </c>
+      <c r="N3" s="2">
+        <v>12</v>
+      </c>
+      <c r="O3" s="2">
+        <v>13</v>
+      </c>
+      <c r="P3" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>15</v>
+      </c>
+      <c r="R3" s="2">
+        <v>16</v>
+      </c>
+      <c r="S3" s="2">
+        <v>17</v>
+      </c>
+      <c r="T3" s="2">
+        <v>18</v>
+      </c>
+      <c r="U3" s="2">
+        <v>19</v>
+      </c>
+      <c r="V3" s="2">
+        <v>20</v>
+      </c>
+      <c r="W3" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f>SUM(C4:W4)</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" ref="B5:B13" si="0">SUM(C5:W5)</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="5">
+        <f>B15</f>
+        <v>140</v>
+      </c>
+      <c r="C14" s="3">
+        <f>B15-SUM(C4:C13)</f>
+        <v>140</v>
+      </c>
+      <c r="D14" s="3">
+        <f>C14-SUM(D4:D13)</f>
+        <v>140</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" ref="E14:W14" si="1">D14-SUM(E4:E13)</f>
+        <v>140</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="O14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="P14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="Q14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="R14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="S14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="T14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="U14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="V14" s="3">
+        <f>U14-SUM(V4:V13)</f>
+        <v>140</v>
+      </c>
+      <c r="W14" s="3">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="10">
+        <f>Tempo!F4</f>
+        <v>140</v>
+      </c>
+      <c r="C15" s="3">
+        <f>B15-B20</f>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="D15" s="3">
+        <f>C15-B20</f>
+        <v>126.66666666666667</v>
+      </c>
+      <c r="E15" s="3">
+        <f>D15-B20</f>
+        <v>120</v>
+      </c>
+      <c r="F15" s="3">
+        <f>E15-B20</f>
+        <v>113.33333333333333</v>
+      </c>
+      <c r="G15" s="3">
+        <f>F15-B20</f>
+        <v>106.66666666666666</v>
+      </c>
+      <c r="H15" s="3">
+        <f>G15-B20</f>
+        <v>99.999999999999986</v>
+      </c>
+      <c r="I15" s="3">
+        <f>H15-B20</f>
+        <v>93.333333333333314</v>
+      </c>
+      <c r="J15" s="3">
+        <f>I15-B20</f>
+        <v>86.666666666666643</v>
+      </c>
+      <c r="K15" s="3">
+        <f>J15-B20</f>
+        <v>79.999999999999972</v>
+      </c>
+      <c r="L15" s="3">
+        <f>K15-B20</f>
+        <v>73.3333333333333</v>
+      </c>
+      <c r="M15" s="3">
+        <f>(L15-B20)</f>
+        <v>66.666666666666629</v>
+      </c>
+      <c r="N15" s="3">
+        <f>M15-B20</f>
+        <v>59.999999999999964</v>
+      </c>
+      <c r="O15" s="3">
+        <f>(N15-B20)</f>
+        <v>53.3333333333333</v>
+      </c>
+      <c r="P15" s="3">
+        <f>(O15-B20)</f>
+        <v>46.666666666666636</v>
+      </c>
+      <c r="Q15" s="3">
+        <f>P15-B20</f>
+        <v>39.999999999999972</v>
+      </c>
+      <c r="R15" s="3">
+        <f>Q15-B20</f>
+        <v>33.333333333333307</v>
+      </c>
+      <c r="S15" s="3">
+        <f>R15-B20</f>
+        <v>26.666666666666639</v>
+      </c>
+      <c r="T15" s="3">
+        <f>S15-B20</f>
+        <v>19.999999999999972</v>
+      </c>
+      <c r="U15" s="3">
+        <f>(T15-B20)</f>
+        <v>13.333333333333304</v>
+      </c>
+      <c r="V15" s="3">
+        <f>U15-B20</f>
+        <v>6.6666666666666368</v>
+      </c>
+      <c r="W15" s="3">
+        <f>IF(V15-B20&lt;0,0,V15-B20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17" s="14"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="12">
+        <f>COUNTA(C3:W3)</f>
+        <v>21</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="11"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="9">
+        <f>B15/B18</f>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T21" s="16"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B24" s="17"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R32" s="16"/>
+    </row>
+    <row r="35" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S35" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:W1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FIX: sprint 3 burndown
</commit_message>
<xml_diff>
--- a/docs/Burndown/Burndown.xlsx
+++ b/docs/Burndown/Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\api-6-semestre\docs\Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528399C4-191F-4448-B7D7-31666D78A026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E96D8E-AE92-4B1B-B9E7-A1A49939BEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2515,7 +2515,7 @@
                   <c:v>3.9400000000000119</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-5.9999999999988063E-2</c:v>
+                  <c:v>1.1990408665951691E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4846,15 +4846,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>256029</xdr:colOff>
+      <xdr:colOff>313179</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>82094</xdr:rowOff>
+      <xdr:rowOff>101144</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>581391</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28941</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>25700</xdr:rowOff>
+      <xdr:rowOff>44750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6970,9 +6970,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34691D87-3A65-488E-9A9A-734FA0D4B672}">
   <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W23" sqref="W23"/>
+      <selection pane="topRight" activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7469,7 +7469,7 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" si="0"/>
-        <v>49.47</v>
+        <v>49.41</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3">
@@ -7529,7 +7529,7 @@
         <v>4</v>
       </c>
       <c r="W13" s="3">
-        <v>4</v>
+        <v>3.94</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -7622,7 +7622,7 @@
       </c>
       <c r="W14" s="3">
         <f t="shared" si="1"/>
-        <v>-5.9999999999988063E-2</v>
+        <v>1.1990408665951691E-14</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixing dates and adding new task time
</commit_message>
<xml_diff>
--- a/docs/Burndown/Burndown.xlsx
+++ b/docs/Burndown/Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\api-6-semestre\docs\Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0EC47E-A295-46ED-855D-96F076B9BEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CD719B-77DE-4CAA-8952-14245CB1C810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1425" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tempo" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="112">
   <si>
     <t>Atividades</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>27/11</t>
+  </si>
+  <si>
+    <t>14/11</t>
   </si>
 </sst>
 </file>
@@ -3330,7 +3333,7 @@
                     <c:v>13/11</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>13/11</c:v>
+                    <c:v>14/11</c:v>
                   </c:pt>
                   <c:pt idx="8">
                     <c:v>15/11</c:v>
@@ -3382,67 +3385,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>148.5</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>147.5</c:v>
+                  <c:v>47.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>143.5</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>143.5</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>143.5</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>143.5</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>143.5</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>143.5</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>143.5</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>143.5</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>143.5</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>143.5</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>143.5</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>143.5</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>143.5</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>143.5</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>143.5</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>143.5</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>143.5</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>143.5</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>143.5</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3565,7 +3568,7 @@
                     <c:v>13/11</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>13/11</c:v>
+                    <c:v>14/11</c:v>
                   </c:pt>
                   <c:pt idx="8">
                     <c:v>15/11</c:v>
@@ -3617,67 +3620,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>142.85714285714286</c:v>
+                  <c:v>47.61904761904762</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>135.71428571428572</c:v>
+                  <c:v>45.238095238095241</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>128.57142857142858</c:v>
+                  <c:v>42.857142857142861</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>121.42857142857144</c:v>
+                  <c:v>40.476190476190482</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>114.28571428571431</c:v>
+                  <c:v>38.095238095238102</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>107.14285714285717</c:v>
+                  <c:v>35.714285714285722</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.00000000000003</c:v>
+                  <c:v>33.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>92.85714285714289</c:v>
+                  <c:v>30.952380952380963</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>85.714285714285751</c:v>
+                  <c:v>28.571428571428584</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>78.571428571428612</c:v>
+                  <c:v>26.190476190476204</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>71.428571428571473</c:v>
+                  <c:v>23.809523809523824</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64.285714285714334</c:v>
+                  <c:v>21.428571428571445</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>57.142857142857189</c:v>
+                  <c:v>19.047619047619065</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>50.000000000000043</c:v>
+                  <c:v>16.666666666666686</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>42.857142857142897</c:v>
+                  <c:v>14.285714285714304</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>35.714285714285751</c:v>
+                  <c:v>11.904761904761923</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28.571428571428608</c:v>
+                  <c:v>9.5238095238095415</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>21.428571428571466</c:v>
+                  <c:v>7.1428571428571601</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14.285714285714324</c:v>
+                  <c:v>4.7619047619047787</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.1428571428571805</c:v>
+                  <c:v>2.3809523809523978</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.730349362740526E-14</c:v>
+                  <c:v>1.6875389974302379E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6611,7 +6614,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6744,11 +6747,11 @@
         <v>42</v>
       </c>
       <c r="N4" s="15">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="O4" s="12">
         <f>N4/7</f>
-        <v>21.428571428571427</v>
+        <v>7.1428571428571432</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -6790,11 +6793,11 @@
       </c>
       <c r="N5" s="12">
         <f>N2*N4</f>
-        <v>7500</v>
+        <v>2500</v>
       </c>
       <c r="O5" s="12">
         <f>N5/7</f>
-        <v>1071.4285714285713</v>
+        <v>357.14285714285717</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -6836,11 +6839,11 @@
       </c>
       <c r="N6" s="12">
         <f>N4*4</f>
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="O6" s="12">
         <f>N6/7</f>
-        <v>85.714285714285708</v>
+        <v>28.571428571428573</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -6882,11 +6885,11 @@
       </c>
       <c r="N7" s="12">
         <f>N5*4</f>
-        <v>30000</v>
+        <v>10000</v>
       </c>
       <c r="O7" s="12">
         <f>N7/7</f>
-        <v>4285.7142857142853</v>
+        <v>1428.5714285714287</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -6928,11 +6931,11 @@
       </c>
       <c r="N8" s="12">
         <f>N4/N9</f>
-        <v>7.1428571428571432</v>
+        <v>2.3809523809523809</v>
       </c>
       <c r="O8" s="12">
         <f>N8/7</f>
-        <v>1.0204081632653061</v>
+        <v>0.3401360544217687</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -9382,7 +9385,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C26" sqref="C26"/>
+      <selection pane="topRight" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9450,7 +9453,7 @@
         <v>97</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>98</v>
@@ -9625,7 +9628,7 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3">
@@ -9638,7 +9641,9 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="3"/>
+      <c r="J6" s="3">
+        <v>1.5</v>
+      </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -9877,91 +9882,91 @@
       </c>
       <c r="B14" s="5">
         <f>B15</f>
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="C14" s="3">
         <f>B15-SUM(C4:C13)</f>
-        <v>148.5</v>
+        <v>48.5</v>
       </c>
       <c r="D14" s="3">
         <f>C14-SUM(D4:D13)</f>
-        <v>147.5</v>
+        <v>47.5</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" ref="E14:W14" si="1">D14-SUM(E4:E13)</f>
-        <v>143.5</v>
+        <v>43.5</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>43.5</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>43.5</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>43.5</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>43.5</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>42</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>42</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>42</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>42</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>42</v>
       </c>
       <c r="O14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>42</v>
       </c>
       <c r="P14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>42</v>
       </c>
       <c r="Q14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>42</v>
       </c>
       <c r="R14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>42</v>
       </c>
       <c r="S14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>42</v>
       </c>
       <c r="T14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>42</v>
       </c>
       <c r="U14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>42</v>
       </c>
       <c r="V14" s="3">
         <f>U14-SUM(V4:V13)</f>
-        <v>143.5</v>
+        <v>42</v>
       </c>
       <c r="W14" s="3">
         <f t="shared" si="1"/>
-        <v>143.5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
@@ -9970,91 +9975,91 @@
       </c>
       <c r="B15" s="10">
         <f>Tempo!N4</f>
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="C15" s="3">
         <f>B15-B20</f>
-        <v>142.85714285714286</v>
+        <v>47.61904761904762</v>
       </c>
       <c r="D15" s="3">
         <f>C15-B20</f>
-        <v>135.71428571428572</v>
+        <v>45.238095238095241</v>
       </c>
       <c r="E15" s="3">
         <f>D15-B20</f>
-        <v>128.57142857142858</v>
+        <v>42.857142857142861</v>
       </c>
       <c r="F15" s="3">
         <f>E15-B20</f>
-        <v>121.42857142857144</v>
+        <v>40.476190476190482</v>
       </c>
       <c r="G15" s="3">
         <f>F15-B20</f>
-        <v>114.28571428571431</v>
+        <v>38.095238095238102</v>
       </c>
       <c r="H15" s="3">
         <f>G15-B20</f>
-        <v>107.14285714285717</v>
+        <v>35.714285714285722</v>
       </c>
       <c r="I15" s="3">
         <f>H15-B20</f>
-        <v>100.00000000000003</v>
+        <v>33.333333333333343</v>
       </c>
       <c r="J15" s="3">
         <f>I15-B20</f>
-        <v>92.85714285714289</v>
+        <v>30.952380952380963</v>
       </c>
       <c r="K15" s="3">
         <f>J15-B20</f>
-        <v>85.714285714285751</v>
+        <v>28.571428571428584</v>
       </c>
       <c r="L15" s="3">
         <f>K15-B20</f>
-        <v>78.571428571428612</v>
+        <v>26.190476190476204</v>
       </c>
       <c r="M15" s="3">
         <f>(L15-B20)</f>
-        <v>71.428571428571473</v>
+        <v>23.809523809523824</v>
       </c>
       <c r="N15" s="3">
         <f>M15-B20</f>
-        <v>64.285714285714334</v>
+        <v>21.428571428571445</v>
       </c>
       <c r="O15" s="3">
         <f>(N15-B20)</f>
-        <v>57.142857142857189</v>
+        <v>19.047619047619065</v>
       </c>
       <c r="P15" s="3">
         <f>(O15-B20)</f>
-        <v>50.000000000000043</v>
+        <v>16.666666666666686</v>
       </c>
       <c r="Q15" s="3">
         <f>P15-B20</f>
-        <v>42.857142857142897</v>
+        <v>14.285714285714304</v>
       </c>
       <c r="R15" s="3">
         <f>Q15-B20</f>
-        <v>35.714285714285751</v>
+        <v>11.904761904761923</v>
       </c>
       <c r="S15" s="3">
         <f>R15-B20</f>
-        <v>28.571428571428608</v>
+        <v>9.5238095238095415</v>
       </c>
       <c r="T15" s="3">
         <f>S15-B20</f>
-        <v>21.428571428571466</v>
+        <v>7.1428571428571601</v>
       </c>
       <c r="U15" s="3">
         <f>(T15-B20)</f>
-        <v>14.285714285714324</v>
+        <v>4.7619047619047787</v>
       </c>
       <c r="V15" s="3">
         <f>U15-B20</f>
-        <v>7.1428571428571805</v>
+        <v>2.3809523809523978</v>
       </c>
       <c r="W15" s="3">
         <f>IF(V15-B20&lt;0,0,V15-B20)</f>
-        <v>3.730349362740526E-14</v>
+        <v>1.6875389974302379E-14</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -10080,7 +10085,7 @@
       </c>
       <c r="B20" s="9">
         <f>B15/B18</f>
-        <v>7.1428571428571432</v>
+        <v>2.3809523809523809</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>